<commit_message>
Build for Jenkins with Testsuite
</commit_message>
<xml_diff>
--- a/CTDC_Automation/TestData/Input_TestData_CanineWorkflow.xlsx
+++ b/CTDC_Automation/TestData/Input_TestData_CanineWorkflow.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laxmi\DemoBuild\DataCommons_Automation\CTDC_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5D6C38-EFE4-41D9-BDBA-F8F003EA15A2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997B9141-9E33-48C8-A180-7846C2752718}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
-    <sheet name="startup" sheetId="1" r:id="rId1"/>
-    <sheet name="testcase" sheetId="2" r:id="rId2"/>
-    <sheet name="Hardcode " sheetId="3" r:id="rId3"/>
+    <sheet name="testcase" sheetId="2" r:id="rId1"/>
+    <sheet name="Hardcode " sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,13 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="118">
-  <si>
-    <t>Environment</t>
-  </si>
-  <si>
-    <t>Url</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="105">
   <si>
     <t>Browser</t>
   </si>
@@ -65,24 +58,6 @@
     <t>propertyvalue</t>
   </si>
   <si>
-    <t>CTDC</t>
-  </si>
-  <si>
-    <t>server</t>
-  </si>
-  <si>
-    <t>user_Id</t>
-  </si>
-  <si>
-    <t>neo4j</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>location_path</t>
-  </si>
-  <si>
     <t>Query</t>
   </si>
   <si>
@@ -365,9 +340,6 @@
     <t>Select_case_checkbox</t>
   </si>
   <si>
-    <t>WebExcel</t>
-  </si>
-  <si>
     <t>MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WITH DISTINCT c AS c, p, s, demo, diag RETURN c.case_id AS `Case ID`, s.clinical_study_designation AS `Study Code`, s.clinical_study_type AS `Study Type`, demo.breed AS Breed, diag.disease_term AS Diagnosis, diag.stage_of_disease AS `Stage of Disease`,demo.patient_age_at_enrollment AS Age, demo.sex AS Sex, demo.neutered_indicator AS `Neutered Status`</t>
   </si>
   <si>
@@ -375,18 +347,6 @@
   </si>
   <si>
     <t>https://caninecommons-stage.cancer.gov/#/cases</t>
-  </si>
-  <si>
-    <t>bolt://ncias-s2261-c.nci.nih.gov:7687</t>
-  </si>
-  <si>
-    <t>R3MtYmJ3W5nHq1W</t>
-  </si>
-  <si>
-    <t>C:\\Data\\Test_outCanine.xlsx</t>
-  </si>
-  <si>
-    <t>C:\\Data\\Test_WebCanine.xlsx</t>
   </si>
 </sst>
 </file>
@@ -758,95 +718,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:H4"/>
-  <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" customWidth="1"/>
-    <col min="4" max="4" width="59.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="70.28515625" customWidth="1"/>
-    <col min="8" max="8" width="28.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>115</v>
-      </c>
-      <c r="G2" t="s">
-        <v>116</v>
-      </c>
-      <c r="H2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D4" s="1"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="http://ncias-q2251-c.nci.nih.gov:7687" xr:uid="{4381B5EF-3CC8-41D8-98D4-CF7F9613D425}"/>
-    <hyperlink ref="B2" r:id="rId2" location="/cases" display="https://caninecommons-stage.cancer.gov/ - /cases" xr:uid="{EE6720A7-C9D8-4EE2-8E31-C0EFEB18C846}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C468257-9521-42A0-A4DB-E0691FA7FE45}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,349 +736,349 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
       <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" t="s">
-        <v>17</v>
-      </c>
       <c r="K1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="K2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" t="s">
-        <v>29</v>
-      </c>
       <c r="K3" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
         <v>73</v>
       </c>
-      <c r="E4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" t="s">
-        <v>81</v>
-      </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J4" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="K4" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
         <v>74</v>
       </c>
-      <c r="D5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" t="s">
-        <v>82</v>
-      </c>
       <c r="H5" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="I5" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J5" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="K5" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" t="s">
         <v>75</v>
       </c>
-      <c r="E6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" t="s">
-        <v>72</v>
-      </c>
-      <c r="H6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" t="s">
-        <v>83</v>
-      </c>
       <c r="K6" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D7" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G7" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="H7" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="I7" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J7" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="K7" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G8" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="H8" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="I8" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J8" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="K8" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G9" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="H9" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="I9" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="J9" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="K9" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G10" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="H10" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="I10" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J10" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1215,7 +1091,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E60AE08-F6F7-4D66-9A20-44C6071A5BA3}">
   <dimension ref="A2:K96"/>
   <sheetViews>
@@ -1236,1205 +1112,1205 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E18" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E35" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F38" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D46" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C50" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" t="s">
+        <v>5</v>
+      </c>
+      <c r="E50" t="s">
+        <v>6</v>
+      </c>
+      <c r="F50" t="s">
+        <v>18</v>
+      </c>
+      <c r="G50" t="s">
+        <v>19</v>
+      </c>
+      <c r="H50" t="s">
+        <v>22</v>
+      </c>
+      <c r="I50" t="s">
+        <v>20</v>
+      </c>
+      <c r="J50" t="s">
         <v>21</v>
       </c>
-      <c r="D50" t="s">
-        <v>7</v>
-      </c>
-      <c r="E50" t="s">
-        <v>8</v>
-      </c>
-      <c r="F50" t="s">
-        <v>26</v>
-      </c>
-      <c r="G50" t="s">
-        <v>27</v>
-      </c>
-      <c r="H50" t="s">
-        <v>30</v>
-      </c>
-      <c r="I50" t="s">
-        <v>28</v>
-      </c>
-      <c r="J50" t="s">
-        <v>29</v>
-      </c>
       <c r="K50" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C51" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" t="s">
+        <v>25</v>
+      </c>
+      <c r="F51" t="s">
+        <v>18</v>
+      </c>
+      <c r="G51" t="s">
+        <v>24</v>
+      </c>
+      <c r="H51" t="s">
+        <v>22</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J51" t="s">
         <v>21</v>
       </c>
-      <c r="D51" t="s">
-        <v>7</v>
-      </c>
-      <c r="E51" t="s">
-        <v>33</v>
-      </c>
-      <c r="F51" t="s">
-        <v>26</v>
-      </c>
-      <c r="G51" t="s">
-        <v>32</v>
-      </c>
-      <c r="H51" t="s">
-        <v>30</v>
-      </c>
-      <c r="I51" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J51" t="s">
-        <v>29</v>
-      </c>
       <c r="K51" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C52" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D52" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E52" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F52" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G52" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="H52" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="J52" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="K52" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C53" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" t="s">
+        <v>5</v>
+      </c>
+      <c r="E53" t="s">
+        <v>25</v>
+      </c>
+      <c r="F53" t="s">
+        <v>18</v>
+      </c>
+      <c r="G53" t="s">
+        <v>24</v>
+      </c>
+      <c r="H53" t="s">
+        <v>22</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J53" t="s">
         <v>21</v>
       </c>
-      <c r="D53" t="s">
-        <v>7</v>
-      </c>
-      <c r="E53" t="s">
-        <v>33</v>
-      </c>
-      <c r="F53" t="s">
-        <v>26</v>
-      </c>
-      <c r="G53" t="s">
-        <v>32</v>
-      </c>
-      <c r="H53" t="s">
-        <v>30</v>
-      </c>
-      <c r="I53" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J53" t="s">
-        <v>29</v>
-      </c>
       <c r="K53" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C54" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" t="s">
+        <v>5</v>
+      </c>
+      <c r="E54" t="s">
+        <v>26</v>
+      </c>
+      <c r="F54" t="s">
+        <v>18</v>
+      </c>
+      <c r="G54" t="s">
+        <v>59</v>
+      </c>
+      <c r="H54" t="s">
+        <v>22</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J54" t="s">
         <v>21</v>
       </c>
-      <c r="D54" t="s">
-        <v>7</v>
-      </c>
-      <c r="E54" t="s">
-        <v>34</v>
-      </c>
-      <c r="F54" t="s">
-        <v>26</v>
-      </c>
-      <c r="G54" t="s">
-        <v>67</v>
-      </c>
-      <c r="H54" t="s">
-        <v>30</v>
-      </c>
-      <c r="I54" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J54" t="s">
-        <v>29</v>
-      </c>
       <c r="K54" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C55" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55" t="s">
+        <v>5</v>
+      </c>
+      <c r="E55" t="s">
+        <v>60</v>
+      </c>
+      <c r="F55" t="s">
+        <v>18</v>
+      </c>
+      <c r="G55" t="s">
+        <v>58</v>
+      </c>
+      <c r="H55" t="s">
+        <v>22</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J55" t="s">
         <v>21</v>
-      </c>
-      <c r="D55" t="s">
-        <v>7</v>
-      </c>
-      <c r="E55" t="s">
-        <v>68</v>
-      </c>
-      <c r="F55" t="s">
-        <v>26</v>
-      </c>
-      <c r="G55" t="s">
-        <v>66</v>
-      </c>
-      <c r="H55" t="s">
-        <v>30</v>
-      </c>
-      <c r="I55" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J55" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C58" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D58" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E58" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F58" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G58" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H58" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="I58" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J58" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K58" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C59" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D59" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E59" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="F59" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G59" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="H59" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="I59" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J59" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K59" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C60" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D60" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E60" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="F60" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G60" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="H60" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="I60" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J60" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K60" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C61" t="s">
+        <v>76</v>
+      </c>
+      <c r="D61" t="s">
+        <v>76</v>
+      </c>
+      <c r="E61" t="s">
         <v>84</v>
       </c>
-      <c r="D61" t="s">
-        <v>84</v>
-      </c>
-      <c r="E61" t="s">
-        <v>92</v>
-      </c>
       <c r="F61" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G61" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="H61" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="I61" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J61" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K61" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B62" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C62" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D62" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E62" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F62" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G62" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="H62" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="I62" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J62" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="K62" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B63" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C63" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D63" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E63" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F63" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G63" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="H63" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="J63" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="K63" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C64" t="s">
+        <v>13</v>
+      </c>
+      <c r="D64" t="s">
+        <v>5</v>
+      </c>
+      <c r="E64" t="s">
+        <v>25</v>
+      </c>
+      <c r="F64" t="s">
+        <v>18</v>
+      </c>
+      <c r="G64" t="s">
+        <v>57</v>
+      </c>
+      <c r="H64" t="s">
+        <v>22</v>
+      </c>
+      <c r="I64" t="s">
+        <v>20</v>
+      </c>
+      <c r="J64" t="s">
         <v>21</v>
       </c>
-      <c r="D64" t="s">
-        <v>7</v>
-      </c>
-      <c r="E64" t="s">
-        <v>33</v>
-      </c>
-      <c r="F64" t="s">
-        <v>26</v>
-      </c>
-      <c r="G64" t="s">
-        <v>65</v>
-      </c>
-      <c r="H64" t="s">
-        <v>30</v>
-      </c>
-      <c r="I64" t="s">
-        <v>28</v>
-      </c>
-      <c r="J64" t="s">
-        <v>29</v>
-      </c>
       <c r="K64" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C65" t="s">
+        <v>13</v>
+      </c>
+      <c r="D65" t="s">
+        <v>5</v>
+      </c>
+      <c r="E65" t="s">
+        <v>6</v>
+      </c>
+      <c r="F65" t="s">
+        <v>18</v>
+      </c>
+      <c r="G65" t="s">
+        <v>58</v>
+      </c>
+      <c r="H65" t="s">
+        <v>22</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J65" t="s">
         <v>21</v>
       </c>
-      <c r="D65" t="s">
-        <v>7</v>
-      </c>
-      <c r="E65" t="s">
-        <v>8</v>
-      </c>
-      <c r="F65" t="s">
-        <v>26</v>
-      </c>
-      <c r="G65" t="s">
-        <v>66</v>
-      </c>
-      <c r="H65" t="s">
-        <v>30</v>
-      </c>
-      <c r="I65" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J65" t="s">
-        <v>29</v>
-      </c>
       <c r="K65" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C66" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D66" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E66" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F66" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G66" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="H66" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C67" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D67" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E67" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F67" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G67" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="H67" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="I67" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J67" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="K67" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C68" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D68" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E68" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F68" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G68" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="H68" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="I68" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J68" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K68" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B69" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C69" t="s">
+        <v>76</v>
+      </c>
+      <c r="D69" t="s">
+        <v>76</v>
+      </c>
+      <c r="E69" t="s">
+        <v>84</v>
+      </c>
+      <c r="F69" t="s">
+        <v>18</v>
+      </c>
+      <c r="G69" t="s">
         <v>93</v>
       </c>
-      <c r="C69" t="s">
-        <v>84</v>
-      </c>
-      <c r="D69" t="s">
-        <v>84</v>
-      </c>
-      <c r="E69" t="s">
-        <v>92</v>
-      </c>
-      <c r="F69" t="s">
-        <v>26</v>
-      </c>
-      <c r="G69" t="s">
-        <v>101</v>
-      </c>
       <c r="H69" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="I69" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J69" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K69" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C70" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D70" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E70" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F70" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G70" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="H70" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="I70" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J70" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K70" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C71" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D71" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E71" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="F71" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G71" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="H71" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="I71" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J71" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K71" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C76" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D76" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
+        <v>81</v>
+      </c>
+      <c r="D77" t="s">
         <v>89</v>
-      </c>
-      <c r="D77" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D78" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C79" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D79" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C80" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D80" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D81" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D82" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C84" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D84" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E84" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F84" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G84" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="H84" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="I84" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J84" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="K84" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C89" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D89" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E89" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="F89" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G89" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="H89" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="I89" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J89" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K89" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C90" t="s">
+        <v>13</v>
+      </c>
+      <c r="D90" t="s">
+        <v>5</v>
+      </c>
+      <c r="E90" t="s">
+        <v>6</v>
+      </c>
+      <c r="F90" t="s">
+        <v>18</v>
+      </c>
+      <c r="G90" t="s">
+        <v>58</v>
+      </c>
+      <c r="H90" t="s">
+        <v>22</v>
+      </c>
+      <c r="I90" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J90" t="s">
         <v>21</v>
       </c>
-      <c r="D90" t="s">
-        <v>7</v>
-      </c>
-      <c r="E90" t="s">
-        <v>8</v>
-      </c>
-      <c r="F90" t="s">
-        <v>26</v>
-      </c>
-      <c r="G90" t="s">
-        <v>66</v>
-      </c>
-      <c r="H90" t="s">
-        <v>30</v>
-      </c>
-      <c r="I90" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J90" t="s">
-        <v>29</v>
-      </c>
       <c r="K90" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C91" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D91" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E91" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="F91" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G91" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="H91" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="I91" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J91" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K91" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C92" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D92" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E92" t="s">
+        <v>81</v>
+      </c>
+      <c r="F92" t="s">
+        <v>18</v>
+      </c>
+      <c r="G92" t="s">
         <v>89</v>
       </c>
-      <c r="F92" t="s">
-        <v>26</v>
-      </c>
-      <c r="G92" t="s">
-        <v>97</v>
-      </c>
       <c r="H92" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="I92" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J92" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K92" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C93" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D93" t="s">
+        <v>65</v>
+      </c>
+      <c r="E93" t="s">
+        <v>20</v>
+      </c>
+      <c r="F93" t="s">
+        <v>20</v>
+      </c>
+      <c r="G93" t="s">
         <v>73</v>
       </c>
-      <c r="E93" t="s">
-        <v>28</v>
-      </c>
-      <c r="F93" t="s">
-        <v>28</v>
-      </c>
-      <c r="G93" t="s">
-        <v>81</v>
-      </c>
       <c r="H93" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="I93" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J93" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="K93" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C94" t="s">
+        <v>66</v>
+      </c>
+      <c r="D94" t="s">
+        <v>69</v>
+      </c>
+      <c r="E94" t="s">
+        <v>20</v>
+      </c>
+      <c r="F94" t="s">
+        <v>20</v>
+      </c>
+      <c r="G94" t="s">
         <v>74</v>
       </c>
-      <c r="D94" t="s">
-        <v>77</v>
-      </c>
-      <c r="E94" t="s">
-        <v>28</v>
-      </c>
-      <c r="F94" t="s">
-        <v>28</v>
-      </c>
-      <c r="G94" t="s">
-        <v>82</v>
-      </c>
       <c r="H94" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="I94" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J94" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="K94" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C95" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D95" t="s">
+        <v>67</v>
+      </c>
+      <c r="E95" t="s">
+        <v>20</v>
+      </c>
+      <c r="F95" t="s">
+        <v>20</v>
+      </c>
+      <c r="G95" t="s">
+        <v>64</v>
+      </c>
+      <c r="H95" t="s">
+        <v>20</v>
+      </c>
+      <c r="I95" t="s">
+        <v>20</v>
+      </c>
+      <c r="J95" t="s">
         <v>75</v>
       </c>
-      <c r="E95" t="s">
-        <v>28</v>
-      </c>
-      <c r="F95" t="s">
-        <v>28</v>
-      </c>
-      <c r="G95" t="s">
-        <v>72</v>
-      </c>
-      <c r="H95" t="s">
-        <v>28</v>
-      </c>
-      <c r="I95" t="s">
-        <v>28</v>
-      </c>
-      <c r="J95" t="s">
-        <v>83</v>
-      </c>
       <c r="K95" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C96" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D96" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="E96" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F96" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G96" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="H96" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="I96" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J96" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="K96" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added functions to: create csv file, read csv file and compare 2 csv files; added relevant jars opencsv and apache comons
</commit_message>
<xml_diff>
--- a/CTDC_Automation/TestData/Input_TestData_CanineWorkflow.xlsx
+++ b/CTDC_Automation/TestData/Input_TestData_CanineWorkflow.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laxmi\DemoBuild\DataCommons_Automation\CTDC_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\DataCommons_Automation\CTDC_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5D6C38-EFE4-41D9-BDBA-F8F003EA15A2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB9A0F7-56C2-4B8D-87F7-1962119D9AE2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="116">
   <si>
     <t>Environment</t>
   </si>
@@ -368,25 +368,19 @@
     <t>WebExcel</t>
   </si>
   <si>
-    <t>MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WITH DISTINCT c AS c, p, s, demo, diag RETURN c.case_id AS `Case ID`, s.clinical_study_designation AS `Study Code`, s.clinical_study_type AS `Study Type`, demo.breed AS Breed, diag.disease_term AS Diagnosis, diag.stage_of_disease AS `Stage of Disease`,demo.patient_age_at_enrollment AS Age, demo.sex AS Sex, demo.neutered_indicator AS `Neutered Status`</t>
-  </si>
-  <si>
-    <t>compare</t>
-  </si>
-  <si>
     <t>https://caninecommons-stage.cancer.gov/#/cases</t>
   </si>
   <si>
-    <t>bolt://ncias-s2261-c.nci.nih.gov:7687</t>
-  </si>
-  <si>
-    <t>R3MtYmJ3W5nHq1W</t>
-  </si>
-  <si>
-    <t>C:\\Data\\Test_outCanine.xlsx</t>
-  </si>
-  <si>
-    <t>C:\\Data\\Test_WebCanine.xlsx</t>
+    <t>C:\Users\radhakrishnang2\Desktop\DataCommons_Automation\CTDC_Automation\TestData\CanineDatafromNeo4j.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\radhakrishnang2\Desktop\DataCommons_Automation\CTDC_Automation\TestData\CanineDataWebData.xlsx</t>
+  </si>
+  <si>
+    <t>http://ncidb-q325-c.nci.nih.gov:7474</t>
+  </si>
+  <si>
+    <t>icdcDBneo4j0</t>
   </si>
 </sst>
 </file>
@@ -439,10 +433,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -761,22 +758,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" customWidth="1"/>
-    <col min="4" max="4" width="59.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="70.28515625" customWidth="1"/>
-    <col min="8" max="8" width="28.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.453125" customWidth="1"/>
+    <col min="4" max="4" width="59.26953125" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="70.26953125" customWidth="1"/>
+    <col min="8" max="8" width="28.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -802,12 +799,12 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -821,19 +818,19 @@
       <c r="F2" t="s">
         <v>115</v>
       </c>
-      <c r="G2" t="s">
-        <v>116</v>
-      </c>
-      <c r="H2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G2" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D4" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="http://ncias-q2251-c.nci.nih.gov:7687" xr:uid="{4381B5EF-3CC8-41D8-98D4-CF7F9613D425}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{4381B5EF-3CC8-41D8-98D4-CF7F9613D425}"/>
     <hyperlink ref="B2" r:id="rId2" location="/cases" display="https://caninecommons-stage.cancer.gov/ - /cases" xr:uid="{EE6720A7-C9D8-4EE2-8E31-C0EFEB18C846}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -843,22 +840,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C468257-9521-42A0-A4DB-E0691FA7FE45}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="76" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.7109375" customWidth="1"/>
-    <col min="7" max="7" width="99.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.7265625" customWidth="1"/>
+    <col min="7" max="7" width="99.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -893,7 +890,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -928,12 +925,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -963,7 +960,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -998,7 +995,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1033,7 +1030,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1068,7 +1065,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1103,7 +1100,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1136,73 +1133,6 @@
       </c>
       <c r="K8" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" t="s">
-        <v>111</v>
-      </c>
-      <c r="J9" t="s">
-        <v>61</v>
-      </c>
-      <c r="K9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" t="s">
-        <v>28</v>
-      </c>
-      <c r="J10" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1223,15 +1153,15 @@
       <selection activeCell="A89" sqref="A89:XFD89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="79.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1248,7 +1178,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>40</v>
       </c>
@@ -1259,7 +1189,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>44</v>
       </c>
@@ -1267,7 +1197,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>46</v>
       </c>
@@ -1275,12 +1205,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D18" t="s">
         <v>42</v>
       </c>
@@ -1288,42 +1218,42 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D21" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D23" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D26" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D27" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D29" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:6" x14ac:dyDescent="0.35">
       <c r="D33" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:6" x14ac:dyDescent="0.35">
       <c r="D34" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:6" x14ac:dyDescent="0.35">
       <c r="D35" t="s">
         <v>55</v>
       </c>
@@ -1331,12 +1261,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:6" x14ac:dyDescent="0.35">
       <c r="D36" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:6" x14ac:dyDescent="0.35">
       <c r="D38" t="s">
         <v>55</v>
       </c>
@@ -1344,27 +1274,27 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:6" x14ac:dyDescent="0.35">
       <c r="D40" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:6" x14ac:dyDescent="0.35">
       <c r="D42" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C45" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:6" x14ac:dyDescent="0.35">
       <c r="D46" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>3</v>
       </c>
@@ -1399,7 +1329,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>3</v>
       </c>
@@ -1434,7 +1364,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>3</v>
       </c>
@@ -1469,7 +1399,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>3</v>
       </c>
@@ -1504,7 +1434,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>3</v>
       </c>
@@ -1539,7 +1469,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>3</v>
       </c>
@@ -1571,7 +1501,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>3</v>
       </c>
@@ -1606,7 +1536,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>3</v>
       </c>
@@ -1641,7 +1571,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>3</v>
       </c>
@@ -1676,7 +1606,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>3</v>
       </c>
@@ -1711,7 +1641,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>28</v>
       </c>
@@ -1746,7 +1676,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>28</v>
       </c>
@@ -1781,7 +1711,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>3</v>
       </c>
@@ -1816,7 +1746,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>3</v>
       </c>
@@ -1851,7 +1781,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>28</v>
       </c>
@@ -1886,7 +1816,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>3</v>
       </c>
@@ -1921,7 +1851,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>3</v>
       </c>
@@ -1956,7 +1886,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>3</v>
       </c>
@@ -1991,7 +1921,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>3</v>
       </c>
@@ -2026,7 +1956,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>3</v>
       </c>
@@ -2061,12 +1991,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C73" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C76" t="s">
         <v>95</v>
       </c>
@@ -2074,7 +2004,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C77" t="s">
         <v>89</v>
       </c>
@@ -2082,7 +2012,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C78" t="s">
         <v>98</v>
       </c>
@@ -2090,7 +2020,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C79" t="s">
         <v>100</v>
       </c>
@@ -2098,7 +2028,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C80" t="s">
         <v>92</v>
       </c>
@@ -2106,7 +2036,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C81" t="s">
         <v>102</v>
       </c>
@@ -2114,7 +2044,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C82" t="s">
         <v>104</v>
       </c>
@@ -2122,7 +2052,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>3</v>
       </c>
@@ -2157,7 +2087,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>3</v>
       </c>
@@ -2192,7 +2122,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>3</v>
       </c>
@@ -2227,7 +2157,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>3</v>
       </c>
@@ -2262,7 +2192,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>3</v>
       </c>
@@ -2297,7 +2227,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>28</v>
       </c>
@@ -2332,7 +2262,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>28</v>
       </c>
@@ -2367,7 +2297,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>28</v>
       </c>
@@ -2402,7 +2332,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Next button fixes and text case and powword files separated
</commit_message>
<xml_diff>
--- a/CTDC_Automation/TestData/Input_TestData_CanineWorkflow.xlsx
+++ b/CTDC_Automation/TestData/Input_TestData_CanineWorkflow.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laxmi\DemoBuild\DataCommons_Automation\CTDC_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laxmi\KatalonApril24\DataCommons_Automation\CTDC_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997B9141-9E33-48C8-A180-7846C2752718}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB428047-3FBF-476C-91B0-5FC27D70DF8C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="110">
   <si>
     <t>Browser</t>
   </si>
@@ -347,6 +347,21 @@
   </si>
   <si>
     <t>https://caninecommons-stage.cancer.gov/#/cases</t>
+  </si>
+  <si>
+    <t>//div[ contains(text(),'Case')]//parent::span//parent::th//parent::tr//parent::thead//parent::table/tbody</t>
+  </si>
+  <si>
+    <t>//div[ contains(text(),'Case')]//parent::span//parent::th//parent::tr//parent::thead//parent::table/thead</t>
+  </si>
+  <si>
+    <t>rowcount</t>
+  </si>
+  <si>
+    <t>G_rowcount</t>
+  </si>
+  <si>
+    <t>19</t>
   </si>
 </sst>
 </file>
@@ -399,10 +414,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -719,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C468257-9521-42A0-A4DB-E0691FA7FE45}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,7 +910,7 @@
         <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>74</v>
+        <v>105</v>
       </c>
       <c r="H5" t="s">
         <v>20</v>
@@ -929,7 +945,7 @@
         <v>20</v>
       </c>
       <c r="G6" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="H6" t="s">
         <v>20</v>
@@ -964,7 +980,7 @@
         <v>20</v>
       </c>
       <c r="G7" t="s">
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="H7" t="s">
         <v>20</v>
@@ -987,10 +1003,10 @@
         <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>107</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>108</v>
       </c>
       <c r="E8" t="s">
         <v>20</v>
@@ -998,8 +1014,8 @@
       <c r="F8" t="s">
         <v>20</v>
       </c>
-      <c r="G8" t="s">
-        <v>20</v>
+      <c r="G8" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="H8" t="s">
         <v>20</v>
@@ -1008,7 +1024,7 @@
         <v>20</v>
       </c>
       <c r="J8" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="K8" t="s">
         <v>12</v>
@@ -1040,10 +1056,10 @@
         <v>20</v>
       </c>
       <c r="I9" t="s">
-        <v>102</v>
+        <v>20</v>
       </c>
       <c r="J9" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="K9" t="s">
         <v>12</v>
@@ -1075,9 +1091,44 @@
         <v>20</v>
       </c>
       <c r="I10" t="s">
-        <v>20</v>
+        <v>102</v>
       </c>
       <c r="J10" t="s">
+        <v>53</v>
+      </c>
+      <c r="K10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" t="s">
         <v>103</v>
       </c>
     </row>

</xml_diff>